<commit_message>
This does not work yet, a bug with multiprocessing and my code is causing it to crash. I will fix it later.
</commit_message>
<xml_diff>
--- a/results/._results.xlsx
+++ b/results/._results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,35 +491,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>193065-1B</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.2473282442748092</v>
+        <v>0.3063467145099799</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1011757347020934</v>
+        <v>0.08730164111955838</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1047169903816835</v>
+        <v>0.08942209365922178</v>
       </c>
       <c r="F2" t="n">
-        <v>0.087074436583873</v>
+        <v>0.07794898112910682</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2416883040454638</v>
+        <v>0.2972049551600615</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1099672004100175</v>
+        <v>0.1034394053193739</v>
       </c>
       <c r="I2" t="n">
-        <v>0.23646931023226</v>
+        <v>0.2252417101770724</v>
       </c>
       <c r="J2" t="n">
-        <v>0.09544167336386078</v>
+        <v>0.08865391294507191</v>
       </c>
       <c r="K2" t="n">
-        <v>26.70343328875996</v>
+        <v>23.01109668093636</v>
       </c>
     </row>
     <row r="3">
@@ -528,35 +528,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>193065-2A</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5820512820512821</v>
+        <v>0.3545537841304748</v>
       </c>
       <c r="D3" t="n">
-        <v>0.07010408162238325</v>
+        <v>0.1238197019414944</v>
       </c>
       <c r="E3" t="n">
-        <v>0.07122789406698471</v>
+        <v>0.1274154204079644</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05683484063202682</v>
+        <v>0.1046758027505544</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5094439136645887</v>
+        <v>0.3198099396192521</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09517692442419252</v>
+        <v>0.1392941611968475</v>
       </c>
       <c r="I3" t="n">
-        <v>0.16991439962817</v>
+        <v>0.2759198469928096</v>
       </c>
       <c r="J3" t="n">
-        <v>0.06535162366870631</v>
+        <v>0.1167975544835497</v>
       </c>
       <c r="K3" t="n">
-        <v>21.79934058714741</v>
+        <v>29.91162840656134</v>
       </c>
     </row>
     <row r="4">
@@ -565,35 +565,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>193065-3A</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.108843537414966</v>
+        <v>0.4753741496598641</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0700546794484702</v>
+        <v>0.09221581389006456</v>
       </c>
       <c r="E4" t="n">
-        <v>0.07042205270050254</v>
+        <v>0.0938088478140727</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0505186818866572</v>
+        <v>0.08106092247733075</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9236125516784897</v>
+        <v>0.4466797907209543</v>
       </c>
       <c r="H4" t="n">
-        <v>0.08326600045975879</v>
+        <v>0.1209698097655999</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1273683862937707</v>
+        <v>0.2313532327563793</v>
       </c>
       <c r="J4" t="n">
-        <v>0.05443018347392521</v>
+        <v>0.09525392531129219</v>
       </c>
       <c r="K4" t="n">
-        <v>20.30704845469804</v>
+        <v>26.54349287132808</v>
       </c>
     </row>
     <row r="5">
@@ -602,35 +602,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R4</t>
+          <t>193065-4</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.549242424242424</v>
+        <v>1.478817733990149</v>
       </c>
       <c r="D5" t="n">
-        <v>0.08028042924718197</v>
+        <v>0.08251425451419704</v>
       </c>
       <c r="E5" t="n">
-        <v>0.07999265717277927</v>
+        <v>0.08350202025488883</v>
       </c>
       <c r="F5" t="n">
-        <v>0.05168196383903029</v>
+        <v>0.05028436604700173</v>
       </c>
       <c r="G5" t="n">
-        <v>1.283588449695047</v>
+        <v>1.20096645139922</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1193211919174486</v>
+        <v>0.1084991357316542</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1529227739626812</v>
+        <v>0.1445935184057397</v>
       </c>
       <c r="J5" t="n">
-        <v>0.06030474992278908</v>
+        <v>0.05618304003900688</v>
       </c>
       <c r="K5" t="n">
-        <v>30.88005741598262</v>
+        <v>25.12896427740401</v>
       </c>
     </row>
     <row r="6">
@@ -639,35 +639,35 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C1</t>
+          <t>193065-5B</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.2441558441558442</v>
+        <v>0.2290160183066362</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1001370420692432</v>
+        <v>0.08741225421308876</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1026211182291094</v>
+        <v>0.09047610520123214</v>
       </c>
       <c r="F6" t="n">
-        <v>0.08968398826331808</v>
+        <v>0.07997078402443927</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2347833936932623</v>
+        <v>0.2205554310404012</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1195221312647571</v>
+        <v>0.1024991225125535</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2494612139124117</v>
+        <v>0.2347428148156322</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1027796986504039</v>
+        <v>0.09044122645761467</v>
       </c>
       <c r="K6" t="n">
-        <v>27.46135539421528</v>
+        <v>25.98222333156137</v>
       </c>
     </row>
     <row r="7">
@@ -676,35 +676,35 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>193065-6B</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9665653495440729</v>
+        <v>0.08343256536370698</v>
       </c>
       <c r="D7" t="n">
-        <v>0.07010036231884058</v>
+        <v>0.1379317473245735</v>
       </c>
       <c r="E7" t="n">
-        <v>0.07196976854462156</v>
+        <v>0.1449745060532031</v>
       </c>
       <c r="F7" t="n">
-        <v>0.05422586004700646</v>
+        <v>0.1286242441130385</v>
       </c>
       <c r="G7" t="n">
-        <v>0.788617771364811</v>
+        <v>0.07283771038901744</v>
       </c>
       <c r="H7" t="n">
-        <v>0.08624195009105211</v>
+        <v>0.1703525330008346</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1442220089767</v>
+        <v>0.4907093426254391</v>
       </c>
       <c r="J7" t="n">
-        <v>0.06075760145905176</v>
+        <v>0.1470139182961846</v>
       </c>
       <c r="K7" t="n">
-        <v>22.99747975411427</v>
+        <v>46.16685410905337</v>
       </c>
     </row>
     <row r="8">
@@ -713,35 +713,35 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>N1</t>
+          <t>193065-7A</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1796875</v>
+        <v>0.2816464406355562</v>
       </c>
       <c r="D8" t="n">
-        <v>0.100040202294686</v>
+        <v>0.1584651034463264</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1033922029601998</v>
+        <v>0.1632208242608844</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0918153615746328</v>
+        <v>0.141525438971844</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1719890625120795</v>
+        <v>0.2556548101770084</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1181472179666918</v>
+        <v>0.1932901674704933</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2719506160155061</v>
+        <v>0.404677649405554</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1042204969475328</v>
+        <v>0.1627206257419432</v>
       </c>
       <c r="K8" t="n">
-        <v>29.82104485393026</v>
+        <v>42.34947294930374</v>
       </c>
     </row>
     <row r="9">
@@ -750,35 +750,35 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>N2</t>
+          <t>193065-8B</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4092827004219409</v>
+        <v>0.4792491643095914</v>
       </c>
       <c r="D9" t="n">
-        <v>0.06997496477455717</v>
+        <v>0.0799988041644204</v>
       </c>
       <c r="E9" t="n">
-        <v>0.07104806242930546</v>
+        <v>0.08106572604861186</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06089031740564841</v>
+        <v>0.07044905478327748</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3777253460517036</v>
+        <v>0.4380812398389292</v>
       </c>
       <c r="H9" t="n">
-        <v>0.08875102137242051</v>
+        <v>0.09692974202509021</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1677264675228566</v>
+        <v>0.1899313395854628</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0703608096680559</v>
+        <v>0.08050470514558757</v>
       </c>
       <c r="K9" t="n">
-        <v>19.8886152169165</v>
+        <v>23.32748775154564</v>
       </c>
     </row>
     <row r="10">
@@ -787,35 +787,35 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>N3</t>
+          <t>193065-9B</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.8813559322033898</v>
+        <v>1.279970381340245</v>
       </c>
       <c r="D10" t="n">
-        <v>0.06998973933172303</v>
+        <v>0.07718992757534039</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0703430761200252</v>
+        <v>0.07769455364855041</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05441577072811794</v>
+        <v>0.06116458108542001</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7302289528715716</v>
+        <v>0.972603047797103</v>
       </c>
       <c r="H10" t="n">
-        <v>0.09145362400365933</v>
+        <v>0.09669634690777239</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1468387739365015</v>
+        <v>0.168562768134817</v>
       </c>
       <c r="J10" t="n">
-        <v>0.06182932255866344</v>
+        <v>0.06882514074071884</v>
       </c>
       <c r="K10" t="n">
-        <v>23.32119296945787</v>
+        <v>30.68623067575896</v>
       </c>
     </row>
     <row r="11">
@@ -824,35 +824,35 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>N4</t>
+          <t>193065-10</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.606382978723404</v>
+        <v>0.3637702503681887</v>
       </c>
       <c r="D11" t="n">
-        <v>0.08004474134460547</v>
+        <v>0.094454080521363</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07984454190864931</v>
+        <v>0.09597324477530572</v>
       </c>
       <c r="F11" t="n">
-        <v>0.05413871220190486</v>
+        <v>0.08296500795287107</v>
       </c>
       <c r="G11" t="n">
-        <v>1.224161851104613</v>
+        <v>0.3443874153212952</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1101630356952656</v>
+        <v>0.1135227495648388</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1498095527679877</v>
+        <v>0.2230626534669266</v>
       </c>
       <c r="J11" t="n">
-        <v>0.06049536187709915</v>
+        <v>0.09419212142604184</v>
       </c>
       <c r="K11" t="n">
-        <v>33.33352633689532</v>
+        <v>26.38823021547552</v>
       </c>
     </row>
     <row r="12">
@@ -861,35 +861,35 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>W1</t>
+          <t>193065-11A</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3.152284263959391</v>
+        <v>0.2866308305878275</v>
       </c>
       <c r="D12" t="n">
-        <v>0.113959460547504</v>
+        <v>0.1135662352264815</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1120730535201965</v>
+        <v>0.1164981045800473</v>
       </c>
       <c r="F12" t="n">
-        <v>0.07957998521258956</v>
+        <v>0.1007517706962739</v>
       </c>
       <c r="G12" t="n">
-        <v>1.538917153961179</v>
+        <v>0.2722031040432004</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1201758186720678</v>
+        <v>0.1370501285870698</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1797840977461756</v>
+        <v>0.282121422990203</v>
       </c>
       <c r="J12" t="n">
-        <v>0.07724338387776326</v>
+        <v>0.1150148850477534</v>
       </c>
       <c r="K12" t="n">
-        <v>101.2563905635704</v>
+        <v>31.59482159921387</v>
       </c>
     </row>
     <row r="13">
@@ -898,35 +898,35 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>208099-CH1</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5.722222222222222</v>
+        <v>0.4174636177139858</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1504722322866344</v>
+        <v>0.05781357724446887</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1470516385702884</v>
+        <v>0.05875669991160901</v>
       </c>
       <c r="F13" t="n">
-        <v>0.09186622969397451</v>
+        <v>0.05057793456123667</v>
       </c>
       <c r="G13" t="n">
-        <v>2.199483705235565</v>
+        <v>0.3777430944927462</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2046686449674033</v>
+        <v>0.06716252801188106</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2501802427306528</v>
+        <v>0.1311880654888385</v>
       </c>
       <c r="J13" t="n">
-        <v>0.09112766868662205</v>
+        <v>0.05704609111816585</v>
       </c>
       <c r="K13" t="n">
-        <v>192.3826452374905</v>
+        <v>16.82733906866358</v>
       </c>
     </row>
     <row r="14">
@@ -935,35 +935,35 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>208099-CH2</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8.631067961165048</v>
+        <v>0.6367920627775899</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1960081018518519</v>
+        <v>0.05889050074943984</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1918169015428574</v>
+        <v>0.05983998765842841</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1069199762361368</v>
+        <v>0.04867937619720036</v>
       </c>
       <c r="G14" t="n">
-        <v>3.04881298535346</v>
+        <v>0.5440673904235515</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2884758767250113</v>
+        <v>0.07071581292737938</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3284019170155369</v>
+        <v>0.1268715298762586</v>
       </c>
       <c r="J14" t="n">
-        <v>0.108165788306071</v>
+        <v>0.05481215847995519</v>
       </c>
       <c r="K14" t="n">
-        <v>287.7882631074611</v>
+        <v>16.51730617726605</v>
       </c>
     </row>
     <row r="15">
@@ -972,34 +972,1773 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>208099-CH3</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.3156492787925565</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.05528476486275092</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.05626621943163217</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.04964595015385867</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.2963037602659832</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.06350802519292131</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.1302811977474765</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.05570360891358057</v>
+      </c>
+      <c r="K15" t="n">
+        <v>16.05882401468993</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>208099-CH4</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.2918701908779752</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.05886369596235874</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.06015751931852843</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0528972810551625</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.2701387415721759</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.06824029356416442</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.1449074411881471</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.05968044190266629</v>
+      </c>
+      <c r="K16" t="n">
+        <v>16.43871247725895</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>208099-CH5</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.4265923568709705</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.05501837627618633</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.05601813130282359</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.04750935270110782</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.3825019741241993</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.06131852911829462</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.1207480879201982</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.05240202844908378</v>
+      </c>
+      <c r="K17" t="n">
+        <v>16.85589668621026</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>208099-CH6</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.224906313249199</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.06395394997293165</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.06533308116944693</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.06020185066774662</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.2130109932219686</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.07696775438993832</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.1717510815091077</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0685967224429134</v>
+      </c>
+      <c r="K18" t="n">
+        <v>18.69634174249987</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>208099-CH7</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.20752235671127</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.07218172277910598</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.07406435529174735</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.06751957183679393</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1969240640209741</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.08417234803394537</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.1876985645040219</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.07575234857854012</v>
+      </c>
+      <c r="K19" t="n">
+        <v>22.86560111889948</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>208099-CH8</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.20752235671127</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.07218172277910598</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.07406435529174735</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.06751957183679393</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1969240640209741</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.08417234803394537</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.1876985645040219</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.07575234857854012</v>
+      </c>
+      <c r="K20" t="n">
+        <v>22.86560111889948</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>208099-CH9</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.4549044995379872</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.06492124134793748</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.06574387138874448</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.05664028992403475</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.4121700724164803</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.07480970479675708</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.1439515844487796</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.06330334668113971</v>
+      </c>
+      <c r="K21" t="n">
+        <v>19.05723794442713</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>208099-CH10</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1.016079874120507</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.05639237628013388</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.05667816379193424</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.04326253396089103</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.7522024681345401</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.06640382185333232</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.1053870844791904</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.04640192554432204</v>
+      </c>
+      <c r="K22" t="n">
+        <v>21.89005717296968</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>208099-CH11</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1.119199618480146</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.06304969995554899</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.06362891713300922</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.04812072014920751</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.8504583792162399</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.07947832144851839</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.1238977543413863</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.05320535057681534</v>
+      </c>
+      <c r="K23" t="n">
+        <v>24.79620526453548</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>208099-CH12</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.8530568842632958</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.04380912927189716</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.04380161428251408</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.03508317880125923</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.6695583069040971</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.05221586669879657</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.08316676406060597</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.03793986355372236</v>
+      </c>
+      <c r="K24" t="n">
+        <v>18.78126538623982</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>208099-CH13</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.6835990083754463</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.06728970595323942</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.06791475097442552</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.05710811473194537</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.5729561227758925</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.07472316883378373</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.1370892858291029</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.06191213105601682</v>
+      </c>
+      <c r="K25" t="n">
+        <v>22.98790859146476</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>208099-CH14</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.8166736136390736</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.06221416527568062</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.06272829928801398</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.05103394078250582</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.6464038991822219</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.06816297110186365</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.1204940203806934</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.0547300728804675</v>
+      </c>
+      <c r="K26" t="n">
+        <v>22.01612453374003</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>208099-CH15</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.4462113491948121</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.06355347123397168</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.06432515013235172</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.05559046682027815</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.4051650958027449</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.07157484674253872</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.1466575779696888</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.06151833807240691</v>
+      </c>
+      <c r="K27" t="n">
+        <v>19.72412344847569</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>208099-CH16</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.8942992870763128</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.06801598304527158</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.06862096390755555</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.05493611441812187</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.7313200313087017</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.08926316243515005</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.1475343526452716</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.06245409430279194</v>
+      </c>
+      <c r="K28" t="n">
+        <v>25.88554405224883</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>208099-CH17</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1.523413966098707</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.07613230933030106</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.07625332177723131</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.05541595390576932</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.13409051217533</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.1026531504242513</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.1484900038481128</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.06215983040683011</v>
+      </c>
+      <c r="K29" t="n">
+        <v>32.63176272684109</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>208099-CH18-90deg</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1.092806880375294</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.0782428740910715</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.07876454729439332</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.06155237797977306</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.8321804283711073</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.1073147870844903</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.1925546491139366</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.0721007627601296</v>
+      </c>
+      <c r="K30" t="n">
+        <v>28.75609194772692</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>208099-CH19</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0.8374372832242412</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.07215314899970465</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.07290189291116392</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.05808453721617515</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.6921083198549681</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.09310023513306261</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.154764735783631</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.06583338850037387</v>
+      </c>
+      <c r="K31" t="n">
+        <v>24.38657551572198</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>208099-CH20</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1.546213592637926</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.06904027050862124</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.06865277077655606</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.05267411602596651</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1.118315454064172</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.09221066343621213</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.1396811639345187</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.05916606176579025</v>
+      </c>
+      <c r="K32" t="n">
+        <v>32.18162205231936</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>208099-CH21</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0.3479427549194993</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.06921308332350865</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0709260729019433</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.06163404406397916</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.3139189677929021</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.08550716858964502</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.1845049213056341</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.07134841933301242</v>
+      </c>
+      <c r="K33" t="n">
+        <v>20.97658530005045</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>216099-BK1</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.2570239844396046</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.08116057759390895</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.08285018670627771</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.07395549370812432</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.2397691673566283</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.09465155557904084</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.2066684765040158</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.0836222510769523</v>
+      </c>
+      <c r="K34" t="n">
+        <v>22.94729335966009</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>216099-BK2</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.2415083311528453</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.07005093733398751</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.07190937972159364</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.06409144334704422</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.2257947694353729</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.08132975362671258</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.1760109587435137</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.07208981258514444</v>
+      </c>
+      <c r="K35" t="n">
+        <v>19.93991756610927</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>216099-BK3</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.2577765755552106</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.07355255675864303</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.07531178763874793</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.06797611257021055</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.2447168727096134</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0.08683314555248633</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.1927891722661753</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.07695286100133535</v>
+      </c>
+      <c r="K36" t="n">
+        <v>21.89236651394393</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>216099-BK4</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0.2534220006469353</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.07029178502851159</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.07212700414603908</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.06517075743771605</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.2306291987242972</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.0838453124325786</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.1864409512365733</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.07403402338739604</v>
+      </c>
+      <c r="K37" t="n">
+        <v>20.06726124646968</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>216099-BK5</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.2574271842565738</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.08058933016347107</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.08228801961009641</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.07436029374823408</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.2410300231612255</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.09430265215811884</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.2012880304119725</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.08391189743897338</v>
+      </c>
+      <c r="K38" t="n">
+        <v>24.17837792825188</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>216099-BK6</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.2020139057152835</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.07939744433130626</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.08150912650377785</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.0742731619354251</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.1875628616376347</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.0935608583478611</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0.2088176197904258</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.08391051093891262</v>
+      </c>
+      <c r="K39" t="n">
+        <v>23.81047453257899</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Lung-1MD2</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0.09549968307627305</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.09171989685027374</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.09631027033289517</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.08520673076139748</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.1706042457406765</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.3684065372658357</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.1149504511057552</v>
+      </c>
+      <c r="K40" t="n">
+        <v>287.8072109054121</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Lung-1LD2</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0.1537138389366693</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.1120853900163747</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.1165818587077811</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.1047526905620423</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.1519855807899402</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.1343430341677353</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.3242768006809282</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.1186228365218494</v>
+      </c>
+      <c r="K41" t="n">
+        <v>33.24996681138243</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Lung-1RD2</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.1076334755111046</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.1133832402824213</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.1180899656717131</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.1061432406569026</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.107472458961546</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.1376314647229725</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.3604284222101862</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.120796816094503</v>
+      </c>
+      <c r="K42" t="n">
+        <v>35.18395312068824</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Reference_C2</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.9665653495440729</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.07002781803542674</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.07192904035716616</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.05420715580231423</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.789498647860758</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.0859447227882303</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.1437040409630082</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.06060569884473403</v>
+      </c>
+      <c r="K43" t="n">
+        <v>22.97284903267187</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Cement_Diffuse</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.4237477185155141</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.1382428079710145</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.1398765665073776</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.1237721026521449</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.3748591807359359</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.2046226919158565</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0.3787278424993986</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.1501956181769875</v>
+      </c>
+      <c r="K44" t="n">
+        <v>44.93275205625682</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Bituminous_Diffuse</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.2534220006469353</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.07029178502851159</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.07212700414603908</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.06517075743771605</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2306291987242972</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.0838453124325786</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.1864409512365733</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.07403402338739604</v>
+      </c>
+      <c r="K45" t="n">
+        <v>20.06726124646968</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Bitumous_Median</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.7276364675621606</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.05920138888888888</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.05977026047587203</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.04965378614700133</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.5964504337034746</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.06767199586071961</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.1238606522538896</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.05437309070680738</v>
+      </c>
+      <c r="K46" t="n">
+        <v>19.78110553666146</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Specular_Pavement</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>2.551189245087901</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.05962843397745572</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.05854517235017831</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.0416256384089698</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1.339036172286537</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.0656589813606389</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.09385653101474643</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.04070878921349885</v>
+      </c>
+      <c r="K47" t="n">
+        <v>42.08364905744622</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Very_dark</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0.5559365623660523</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.03711757397342996</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.03735446324928758</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.03139402046797896</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.475286229635129</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.04156999568865775</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.07335443123557273</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.03397497248047825</v>
+      </c>
+      <c r="K48" t="n">
+        <v>11.12187887523656</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>R1</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0.2473282442748092</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.1011757347020934</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.1047169903816835</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.087074436583873</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.2416883040454638</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.1099672004100175</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.23646931023226</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.09544167336386078</v>
+      </c>
+      <c r="K49" t="n">
+        <v>26.70343328875996</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0.5820512820512821</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.07010408162238325</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.07122789406698471</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.05683484063202682</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.5094439136645887</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.09517692442419252</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.16991439962817</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.06535162366870631</v>
+      </c>
+      <c r="K50" t="n">
+        <v>21.79934058714741</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>R3</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>1.108843537414966</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0700546794484702</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.07042205270050254</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.0505186818866572</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.9236125516784897</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.08326600045975879</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.1273683862937707</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.05443018347392521</v>
+      </c>
+      <c r="K51" t="n">
+        <v>20.30704845469804</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>R4</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1.549242424242424</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.08028042924718197</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.07999265717277927</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.05168196383903029</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1.283588449695047</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.1193211919174486</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.1529227739626812</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.06030474992278908</v>
+      </c>
+      <c r="K52" t="n">
+        <v>30.88005741598262</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0.2441558441558442</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.1001370420692432</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.1026211182291094</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.08968398826331808</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.2347833936932623</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.1195221312647571</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.2494612139124117</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.1027796986504039</v>
+      </c>
+      <c r="K53" t="n">
+        <v>27.46135539421528</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0.9665653495440729</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.07010036231884058</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.07196976854462156</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.05422586004700646</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.788617771364811</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.08624195009105211</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.1442220089767</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.06075760145905176</v>
+      </c>
+      <c r="K54" t="n">
+        <v>22.99747975411427</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>N1</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0.1796875</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.100040202294686</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.1033922029601998</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.0918153615746328</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.1719890625120795</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.1181472179666918</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.2719506160155061</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.1042204969475328</v>
+      </c>
+      <c r="K55" t="n">
+        <v>29.82104485393026</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>N2</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0.4092827004219409</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.06997496477455717</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.07104806242930546</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.06089031740564841</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.3777253460517036</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.08875102137242051</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.1677264675228566</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.0703608096680559</v>
+      </c>
+      <c r="K56" t="n">
+        <v>19.8886152169165</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>N3</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0.8813559322033898</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.06998973933172303</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.0703430761200252</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.05441577072811794</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.7302289528715716</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.09145362400365933</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.1468387739365015</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.06182932255866344</v>
+      </c>
+      <c r="K57" t="n">
+        <v>23.32119296945787</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>N4</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1.606382978723404</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.08004474134460547</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.07984454190864931</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.05413871220190486</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.224161851104613</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.1101630356952656</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.1498095527679877</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.06049536187709915</v>
+      </c>
+      <c r="K58" t="n">
+        <v>33.33352633689532</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>W1</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>3.152284263959391</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.113959460547504</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.1120730535201965</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.07957998521258956</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1.538917153961179</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.1201758186720678</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.1797840977461756</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.07724338387776326</v>
+      </c>
+      <c r="K59" t="n">
+        <v>101.2563905635704</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>W2</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>5.722222222222222</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.1504722322866344</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.1470516385702884</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.09186622969397451</v>
+      </c>
+      <c r="G60" t="n">
+        <v>2.199483705235565</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.2046686449674033</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.2501802427306528</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.09112766868662205</v>
+      </c>
+      <c r="K60" t="n">
+        <v>192.3826452374905</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>W3</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>8.631067961165048</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.1960081018518519</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.1918169015428574</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.1069199762361368</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3.04881298535346</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.2884758767250113</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.3284019170155369</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.108165788306071</v>
+      </c>
+      <c r="K61" t="n">
+        <v>287.7882631074611</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>W4</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C62" t="n">
         <v>10.83802816901408</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D62" t="n">
         <v>0.2470572916666667</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E62" t="n">
         <v>0.2386854152655057</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F62" t="n">
         <v>0.1160306569847246</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G62" t="n">
         <v>3.902628952874985</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H62" t="n">
         <v>8.812300595121476</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I62" t="n">
         <v>8.234964100988691</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J62" t="n">
         <v>2.082009142850571</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K62" t="n">
         <v>12807.26522110153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored some code, added Q-table representation (still needs fixing)
</commit_message>
<xml_diff>
--- a/results/._results.xlsx
+++ b/results/._results.xlsx
@@ -507,19 +507,19 @@
         <v>0.07794898112910682</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2972049551600615</v>
+        <v>0.2972456658126977</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1034394053193739</v>
+        <v>0.1033148979513702</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2252417101770724</v>
+        <v>0.2040315424866941</v>
       </c>
       <c r="J2" t="n">
-        <v>0.08865391294507191</v>
+        <v>0.08795209996197356</v>
       </c>
       <c r="K2" t="n">
-        <v>23.01109668093636</v>
+        <v>20.13955931962898</v>
       </c>
     </row>
     <row r="3">
@@ -544,19 +544,19 @@
         <v>0.1046758027505544</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3198099396192521</v>
+        <v>0.3202090205477859</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1392941611968475</v>
+        <v>0.141135510571515</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2759198469928096</v>
+        <v>0.2469009875247964</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1167975544835497</v>
+        <v>0.1167165657040767</v>
       </c>
       <c r="K3" t="n">
-        <v>29.91162840656134</v>
+        <v>26.28545967538618</v>
       </c>
     </row>
     <row r="4">
@@ -581,19 +581,19 @@
         <v>0.08106092247733075</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4466797907209543</v>
+        <v>0.4471719605576131</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1209698097655999</v>
+        <v>0.1245082554597461</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2313532327563793</v>
+        <v>0.2098126904736013</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09525392531129219</v>
+        <v>0.09555469814452291</v>
       </c>
       <c r="K4" t="n">
-        <v>26.54349287132808</v>
+        <v>23.81667576418965</v>
       </c>
     </row>
     <row r="5">
@@ -618,19 +618,19 @@
         <v>0.05028436604700173</v>
       </c>
       <c r="G5" t="n">
-        <v>1.20096645139922</v>
+        <v>1.202042913278424</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1084991357316542</v>
+        <v>0.1195192073572442</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1445935184057397</v>
+        <v>0.1443074498283486</v>
       </c>
       <c r="J5" t="n">
-        <v>0.05618304003900688</v>
+        <v>0.05887567993940658</v>
       </c>
       <c r="K5" t="n">
-        <v>25.12896427740401</v>
+        <v>25.1752473420393</v>
       </c>
     </row>
     <row r="6">
@@ -655,19 +655,19 @@
         <v>0.07997078402443927</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2205554310404012</v>
+        <v>0.2211982898713656</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1024991225125535</v>
+        <v>0.1007340604254252</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2347428148156322</v>
+        <v>0.2096324317724268</v>
       </c>
       <c r="J6" t="n">
-        <v>0.09044122645761467</v>
+        <v>0.08917070744318134</v>
       </c>
       <c r="K6" t="n">
-        <v>25.98222333156137</v>
+        <v>23.19186666482543</v>
       </c>
     </row>
     <row r="7">
@@ -692,19 +692,19 @@
         <v>0.1286242441130385</v>
       </c>
       <c r="G7" t="n">
-        <v>0.07283771038901744</v>
+        <v>0.07285294065657023</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1703525330008346</v>
+        <v>0.1648544591774143</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4907093426254391</v>
+        <v>0.4599569950780482</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1470139182961846</v>
+        <v>0.1432047580746728</v>
       </c>
       <c r="K7" t="n">
-        <v>46.16685410905337</v>
+        <v>43.11997719399789</v>
       </c>
     </row>
     <row r="8">
@@ -729,19 +729,19 @@
         <v>0.141525438971844</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2556548101770084</v>
+        <v>0.2557834241077624</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1932901674704933</v>
+        <v>0.1937117009263358</v>
       </c>
       <c r="I8" t="n">
-        <v>0.404677649405554</v>
+        <v>0.3616825290241982</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1627206257419432</v>
+        <v>0.1611675782607686</v>
       </c>
       <c r="K8" t="n">
-        <v>42.34947294930374</v>
+        <v>37.03640192633746</v>
       </c>
     </row>
     <row r="9">
@@ -766,19 +766,19 @@
         <v>0.07044905478327748</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4380812398389292</v>
+        <v>0.4383889395381523</v>
       </c>
       <c r="H9" t="n">
-        <v>0.09692974202509021</v>
+        <v>0.09866381709980694</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1899313395854628</v>
+        <v>0.170554904301805</v>
       </c>
       <c r="J9" t="n">
-        <v>0.08050470514558757</v>
+        <v>0.08055007163171944</v>
       </c>
       <c r="K9" t="n">
-        <v>23.32748775154564</v>
+        <v>20.62937331895894</v>
       </c>
     </row>
     <row r="10">
@@ -803,19 +803,19 @@
         <v>0.06116458108542001</v>
       </c>
       <c r="G10" t="n">
-        <v>0.972603047797103</v>
+        <v>0.9746215328667083</v>
       </c>
       <c r="H10" t="n">
-        <v>0.09669634690777239</v>
+        <v>0.1025977156603644</v>
       </c>
       <c r="I10" t="n">
-        <v>0.168562768134817</v>
+        <v>0.1580951150586264</v>
       </c>
       <c r="J10" t="n">
-        <v>0.06882514074071884</v>
+        <v>0.07052134202038196</v>
       </c>
       <c r="K10" t="n">
-        <v>30.68623067575896</v>
+        <v>29.39700452264977</v>
       </c>
     </row>
     <row r="11">
@@ -840,19 +840,19 @@
         <v>0.08296500795287107</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3443874153212952</v>
+        <v>0.3443110007680696</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1135227495648388</v>
+        <v>0.1156889325695743</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2230626534669266</v>
+        <v>0.1985400232499905</v>
       </c>
       <c r="J11" t="n">
-        <v>0.09419212142604184</v>
+        <v>0.09412716128798414</v>
       </c>
       <c r="K11" t="n">
-        <v>26.38823021547552</v>
+        <v>23.06011571558463</v>
       </c>
     </row>
     <row r="12">
@@ -877,19 +877,19 @@
         <v>0.1007517706962739</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2722031040432004</v>
+        <v>0.2722390571463106</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1370501285870698</v>
+        <v>0.1386271122784152</v>
       </c>
       <c r="I12" t="n">
-        <v>0.282121422990203</v>
+        <v>0.2515429630026768</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1150148850477534</v>
+        <v>0.1146197168860528</v>
       </c>
       <c r="K12" t="n">
-        <v>31.59482159921387</v>
+        <v>27.87586356053934</v>
       </c>
     </row>
     <row r="13">
@@ -914,19 +914,19 @@
         <v>0.05057793456123667</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3777430944927462</v>
+        <v>0.3779937184996928</v>
       </c>
       <c r="H13" t="n">
-        <v>0.06716252801188106</v>
+        <v>0.0676809140086575</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1311880654888385</v>
+        <v>0.1151514624294538</v>
       </c>
       <c r="J13" t="n">
-        <v>0.05704609111816585</v>
+        <v>0.05678924641479483</v>
       </c>
       <c r="K13" t="n">
-        <v>16.82733906866358</v>
+        <v>14.75183352887103</v>
       </c>
     </row>
     <row r="14">
@@ -951,19 +951,19 @@
         <v>0.04867937619720036</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5440673904235515</v>
+        <v>0.5443120019067434</v>
       </c>
       <c r="H14" t="n">
-        <v>0.07071581292737938</v>
+        <v>0.07350784200384181</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1268715298762586</v>
+        <v>0.1145959467730113</v>
       </c>
       <c r="J14" t="n">
-        <v>0.05481215847995519</v>
+        <v>0.05528269754617164</v>
       </c>
       <c r="K14" t="n">
-        <v>16.51730617726605</v>
+        <v>14.94179469836018</v>
       </c>
     </row>
     <row r="15">
@@ -988,19 +988,19 @@
         <v>0.04964595015385867</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2963037602659832</v>
+        <v>0.2964947085670804</v>
       </c>
       <c r="H15" t="n">
-        <v>0.06350802519292131</v>
+        <v>0.06308050363147635</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1302811977474765</v>
+        <v>0.1150581422383133</v>
       </c>
       <c r="J15" t="n">
-        <v>0.05570360891358057</v>
+        <v>0.05518829081207459</v>
       </c>
       <c r="K15" t="n">
-        <v>16.05882401468993</v>
+        <v>14.09304395399147</v>
       </c>
     </row>
     <row r="16">
@@ -1025,19 +1025,19 @@
         <v>0.0528972810551625</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2701387415721759</v>
+        <v>0.2702920638548952</v>
       </c>
       <c r="H16" t="n">
-        <v>0.06824029356416442</v>
+        <v>0.06764090875841237</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1449074411881471</v>
+        <v>0.1290495609894066</v>
       </c>
       <c r="J16" t="n">
-        <v>0.05968044190266629</v>
+        <v>0.05906338732167066</v>
       </c>
       <c r="K16" t="n">
-        <v>16.43871247725895</v>
+        <v>14.39227386417705</v>
       </c>
     </row>
     <row r="17">
@@ -1062,19 +1062,19 @@
         <v>0.04750935270110782</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3825019741241993</v>
+        <v>0.3828003039143199</v>
       </c>
       <c r="H17" t="n">
-        <v>0.06131852911829462</v>
+        <v>0.0617971423189448</v>
       </c>
       <c r="I17" t="n">
-        <v>0.1207480879201982</v>
+        <v>0.1063800241257137</v>
       </c>
       <c r="J17" t="n">
-        <v>0.05240202844908378</v>
+        <v>0.05227561226434256</v>
       </c>
       <c r="K17" t="n">
-        <v>16.85589668621026</v>
+        <v>15.11060575074197</v>
       </c>
     </row>
     <row r="18">
@@ -1099,19 +1099,19 @@
         <v>0.06020185066774662</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2130109932219686</v>
+        <v>0.2130925048614002</v>
       </c>
       <c r="H18" t="n">
-        <v>0.07696775438993832</v>
+        <v>0.07524816229733493</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1717510815091077</v>
+        <v>0.152752599799113</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0685967224429134</v>
+        <v>0.06739125100617357</v>
       </c>
       <c r="K18" t="n">
-        <v>18.69634174249987</v>
+        <v>16.26050190694349</v>
       </c>
     </row>
     <row r="19">
@@ -1136,19 +1136,19 @@
         <v>0.06751957183679393</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1969240640209741</v>
+        <v>0.1970577619657727</v>
       </c>
       <c r="H19" t="n">
-        <v>0.08417234803394537</v>
+        <v>0.08196091364460469</v>
       </c>
       <c r="I19" t="n">
-        <v>0.1876985645040219</v>
+        <v>0.1643843896208524</v>
       </c>
       <c r="J19" t="n">
-        <v>0.07575234857854012</v>
+        <v>0.0743049060016075</v>
       </c>
       <c r="K19" t="n">
-        <v>22.86560111889948</v>
+        <v>20.12952073901175</v>
       </c>
     </row>
     <row r="20">
@@ -1173,19 +1173,19 @@
         <v>0.06751957183679393</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1969240640209741</v>
+        <v>0.1970577619657727</v>
       </c>
       <c r="H20" t="n">
-        <v>0.08417234803394537</v>
+        <v>0.08196091364460469</v>
       </c>
       <c r="I20" t="n">
-        <v>0.1876985645040219</v>
+        <v>0.1643843896208524</v>
       </c>
       <c r="J20" t="n">
-        <v>0.07575234857854012</v>
+        <v>0.0743049060016075</v>
       </c>
       <c r="K20" t="n">
-        <v>22.86560111889948</v>
+        <v>20.12952073901175</v>
       </c>
     </row>
     <row r="21">
@@ -1210,19 +1210,19 @@
         <v>0.05664028992403475</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4121700724164803</v>
+        <v>0.4123634543911418</v>
       </c>
       <c r="H21" t="n">
-        <v>0.07480970479675708</v>
+        <v>0.07590889011216136</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1439515844487796</v>
+        <v>0.1267059362571569</v>
       </c>
       <c r="J21" t="n">
-        <v>0.06330334668113971</v>
+        <v>0.06330966339234761</v>
       </c>
       <c r="K21" t="n">
-        <v>19.05723794442713</v>
+        <v>16.74112268356304</v>
       </c>
     </row>
     <row r="22">
@@ -1247,19 +1247,19 @@
         <v>0.04326253396089103</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7522024681345401</v>
+        <v>0.7522369092498352</v>
       </c>
       <c r="H22" t="n">
-        <v>0.06640382185333232</v>
+        <v>0.07124799307806935</v>
       </c>
       <c r="I22" t="n">
-        <v>0.1053870844791904</v>
+        <v>0.09745082829492657</v>
       </c>
       <c r="J22" t="n">
-        <v>0.04640192554432204</v>
+        <v>0.04768195187944564</v>
       </c>
       <c r="K22" t="n">
-        <v>21.89005717296968</v>
+        <v>20.87265445074505</v>
       </c>
     </row>
     <row r="23">
@@ -1284,19 +1284,19 @@
         <v>0.04812072014920751</v>
       </c>
       <c r="G23" t="n">
-        <v>0.8504583792162399</v>
+        <v>0.8502339099003428</v>
       </c>
       <c r="H23" t="n">
-        <v>0.07947832144851839</v>
+        <v>0.0854531856976482</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1238977543413863</v>
+        <v>0.1168563184955383</v>
       </c>
       <c r="J23" t="n">
-        <v>0.05320535057681534</v>
+        <v>0.0547648148681523</v>
       </c>
       <c r="K23" t="n">
-        <v>24.79620526453548</v>
+        <v>23.86384542620292</v>
       </c>
     </row>
     <row r="24">
@@ -1321,19 +1321,19 @@
         <v>0.03508317880125923</v>
       </c>
       <c r="G24" t="n">
-        <v>0.6695583069040971</v>
+        <v>0.6697817020367801</v>
       </c>
       <c r="H24" t="n">
-        <v>0.05221586669879657</v>
+        <v>0.0562394828882769</v>
       </c>
       <c r="I24" t="n">
-        <v>0.08316676406060597</v>
+        <v>0.0759885262705408</v>
       </c>
       <c r="J24" t="n">
-        <v>0.03793986355372236</v>
+        <v>0.03914603498293835</v>
       </c>
       <c r="K24" t="n">
-        <v>18.78126538623982</v>
+        <v>17.78134738810562</v>
       </c>
     </row>
     <row r="25">
@@ -1358,19 +1358,19 @@
         <v>0.05710811473194537</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5729561227758925</v>
+        <v>0.5732235773387598</v>
       </c>
       <c r="H25" t="n">
-        <v>0.07472316883378373</v>
+        <v>0.07684722364864731</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1370892858291029</v>
+        <v>0.1204982377153997</v>
       </c>
       <c r="J25" t="n">
-        <v>0.06191213105601682</v>
+        <v>0.06243296276890184</v>
       </c>
       <c r="K25" t="n">
-        <v>22.98790859146476</v>
+        <v>20.92494562804425</v>
       </c>
     </row>
     <row r="26">
@@ -1395,19 +1395,19 @@
         <v>0.05103394078250582</v>
       </c>
       <c r="G26" t="n">
-        <v>0.6464038991822219</v>
+        <v>0.6466105726898478</v>
       </c>
       <c r="H26" t="n">
-        <v>0.06816297110186365</v>
+        <v>0.07069640728971914</v>
       </c>
       <c r="I26" t="n">
-        <v>0.1204940203806934</v>
+        <v>0.1072110374411715</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0547300728804675</v>
+        <v>0.05535281918381674</v>
       </c>
       <c r="K26" t="n">
-        <v>22.01612453374003</v>
+        <v>20.42878162282372</v>
       </c>
     </row>
     <row r="27">
@@ -1432,19 +1432,19 @@
         <v>0.05559046682027815</v>
       </c>
       <c r="G27" t="n">
-        <v>0.4051650958027449</v>
+        <v>0.4053671381841266</v>
       </c>
       <c r="H27" t="n">
-        <v>0.07157484674253872</v>
+        <v>0.07213087494359306</v>
       </c>
       <c r="I27" t="n">
-        <v>0.1466575779696888</v>
+        <v>0.1324034257326203</v>
       </c>
       <c r="J27" t="n">
-        <v>0.06151833807240691</v>
+        <v>0.06145028511876537</v>
       </c>
       <c r="K27" t="n">
-        <v>19.72412344847569</v>
+        <v>17.86908198103261</v>
       </c>
     </row>
     <row r="28">
@@ -1469,19 +1469,19 @@
         <v>0.05493611441812187</v>
       </c>
       <c r="G28" t="n">
-        <v>0.7313200313087017</v>
+        <v>0.731677917352567</v>
       </c>
       <c r="H28" t="n">
-        <v>0.08926316243515005</v>
+        <v>0.09573836041154497</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1475343526452716</v>
+        <v>0.1363913802448938</v>
       </c>
       <c r="J28" t="n">
-        <v>0.06245409430279194</v>
+        <v>0.06418174036971154</v>
       </c>
       <c r="K28" t="n">
-        <v>25.88554405224883</v>
+        <v>24.35962636319091</v>
       </c>
     </row>
     <row r="29">
@@ -1506,19 +1506,19 @@
         <v>0.05541595390576932</v>
       </c>
       <c r="G29" t="n">
-        <v>1.13409051217533</v>
+        <v>1.133420146561067</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1026531504242513</v>
+        <v>0.1120514500942302</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1484900038481128</v>
+        <v>0.1421073723629031</v>
       </c>
       <c r="J29" t="n">
-        <v>0.06215983040683011</v>
+        <v>0.06473357145064748</v>
       </c>
       <c r="K29" t="n">
-        <v>32.63176272684109</v>
+        <v>31.77254005508295</v>
       </c>
     </row>
     <row r="30">
@@ -1543,19 +1543,19 @@
         <v>0.06155237797977306</v>
       </c>
       <c r="G30" t="n">
-        <v>0.8321804283711073</v>
+        <v>0.8359301777940167</v>
       </c>
       <c r="H30" t="n">
-        <v>0.1073147870844903</v>
+        <v>0.1151238718838698</v>
       </c>
       <c r="I30" t="n">
-        <v>0.1925546491139366</v>
+        <v>0.1858667257491449</v>
       </c>
       <c r="J30" t="n">
-        <v>0.0721007627601296</v>
+        <v>0.07431036494575549</v>
       </c>
       <c r="K30" t="n">
-        <v>28.75609194772692</v>
+        <v>27.9379142829445</v>
       </c>
     </row>
     <row r="31">
@@ -1580,19 +1580,19 @@
         <v>0.05808453721617515</v>
       </c>
       <c r="G31" t="n">
-        <v>0.6921083198549681</v>
+        <v>0.6923038755458126</v>
       </c>
       <c r="H31" t="n">
-        <v>0.09310023513306261</v>
+        <v>0.09923951130954224</v>
       </c>
       <c r="I31" t="n">
-        <v>0.154764735783631</v>
+        <v>0.1422803974581673</v>
       </c>
       <c r="J31" t="n">
-        <v>0.06583338850037387</v>
+        <v>0.06731659250363188</v>
       </c>
       <c r="K31" t="n">
-        <v>24.38657551572198</v>
+        <v>22.77731077002257</v>
       </c>
     </row>
     <row r="32">
@@ -1617,19 +1617,19 @@
         <v>0.05267411602596651</v>
       </c>
       <c r="G32" t="n">
-        <v>1.118315454064172</v>
+        <v>1.117706282932193</v>
       </c>
       <c r="H32" t="n">
-        <v>0.09221066343621213</v>
+        <v>0.09946768686087219</v>
       </c>
       <c r="I32" t="n">
-        <v>0.1396811639345187</v>
+        <v>0.1309833084302516</v>
       </c>
       <c r="J32" t="n">
-        <v>0.05916606176579025</v>
+        <v>0.06115321744243386</v>
       </c>
       <c r="K32" t="n">
-        <v>32.18162205231936</v>
+        <v>31.19531759062696</v>
       </c>
     </row>
     <row r="33">
@@ -1654,19 +1654,19 @@
         <v>0.06163404406397916</v>
       </c>
       <c r="G33" t="n">
-        <v>0.3139189677929021</v>
+        <v>0.3146092646010418</v>
       </c>
       <c r="H33" t="n">
-        <v>0.08550716858964502</v>
+        <v>0.08686675875844448</v>
       </c>
       <c r="I33" t="n">
-        <v>0.1845049213056341</v>
+        <v>0.1679039311335213</v>
       </c>
       <c r="J33" t="n">
-        <v>0.07134841933301242</v>
+        <v>0.0713912523817984</v>
       </c>
       <c r="K33" t="n">
-        <v>20.97658530005045</v>
+        <v>19.0439927792589</v>
       </c>
     </row>
     <row r="34">
@@ -1691,19 +1691,19 @@
         <v>0.07395549370812432</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2397691673566283</v>
+        <v>0.2398727774251339</v>
       </c>
       <c r="H34" t="n">
-        <v>0.09465155557904084</v>
+        <v>0.09308577671590609</v>
       </c>
       <c r="I34" t="n">
-        <v>0.2066684765040158</v>
+        <v>0.1842297969013482</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0836222510769523</v>
+        <v>0.08237298218835001</v>
       </c>
       <c r="K34" t="n">
-        <v>22.94729335966009</v>
+        <v>20.05437592956093</v>
       </c>
     </row>
     <row r="35">
@@ -1728,19 +1728,19 @@
         <v>0.06409144334704422</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2257947694353729</v>
+        <v>0.225930098905363</v>
       </c>
       <c r="H35" t="n">
-        <v>0.08132975362671258</v>
+        <v>0.07992035905947019</v>
       </c>
       <c r="I35" t="n">
-        <v>0.1760109587435137</v>
+        <v>0.155465753515002</v>
       </c>
       <c r="J35" t="n">
-        <v>0.07208981258514444</v>
+        <v>0.07104449733033055</v>
       </c>
       <c r="K35" t="n">
-        <v>19.93991756610927</v>
+        <v>17.32108462633394</v>
       </c>
     </row>
     <row r="36">
@@ -1765,19 +1765,19 @@
         <v>0.06797611257021055</v>
       </c>
       <c r="G36" t="n">
-        <v>0.2447168727096134</v>
+        <v>0.2448692647797002</v>
       </c>
       <c r="H36" t="n">
-        <v>0.08683314555248633</v>
+        <v>0.08521707835292583</v>
       </c>
       <c r="I36" t="n">
-        <v>0.1927891722661753</v>
+        <v>0.1707419077817861</v>
       </c>
       <c r="J36" t="n">
-        <v>0.07695286100133535</v>
+        <v>0.0757762544038694</v>
       </c>
       <c r="K36" t="n">
-        <v>21.89236651394393</v>
+        <v>19.10065369771936</v>
       </c>
     </row>
     <row r="37">
@@ -1802,19 +1802,19 @@
         <v>0.06517075743771605</v>
       </c>
       <c r="G37" t="n">
-        <v>0.2306291987242972</v>
+        <v>0.2307169350353097</v>
       </c>
       <c r="H37" t="n">
-        <v>0.0838453124325786</v>
+        <v>0.08263204119155582</v>
       </c>
       <c r="I37" t="n">
-        <v>0.1864409512365733</v>
+        <v>0.1670756976252482</v>
       </c>
       <c r="J37" t="n">
-        <v>0.07403402338739604</v>
+        <v>0.07310974437270988</v>
       </c>
       <c r="K37" t="n">
-        <v>20.06726124646968</v>
+        <v>17.61315680424924</v>
       </c>
     </row>
     <row r="38">
@@ -1839,19 +1839,19 @@
         <v>0.07436029374823408</v>
       </c>
       <c r="G38" t="n">
-        <v>0.2410300231612255</v>
+        <v>0.2412039202699424</v>
       </c>
       <c r="H38" t="n">
-        <v>0.09430265215811884</v>
+        <v>0.09279250341594186</v>
       </c>
       <c r="I38" t="n">
-        <v>0.2012880304119725</v>
+        <v>0.1758614828727577</v>
       </c>
       <c r="J38" t="n">
-        <v>0.08391189743897338</v>
+        <v>0.08278253328107571</v>
       </c>
       <c r="K38" t="n">
-        <v>24.17837792825188</v>
+        <v>20.9274919615236</v>
       </c>
     </row>
     <row r="39">
@@ -1876,19 +1876,19 @@
         <v>0.0742731619354251</v>
       </c>
       <c r="G39" t="n">
-        <v>0.1875628616376347</v>
+        <v>0.1876725652403878</v>
       </c>
       <c r="H39" t="n">
-        <v>0.0935608583478611</v>
+        <v>0.09112732142778837</v>
       </c>
       <c r="I39" t="n">
-        <v>0.2088176197904258</v>
+        <v>0.1830448203153128</v>
       </c>
       <c r="J39" t="n">
-        <v>0.08391051093891262</v>
+        <v>0.08229232898566517</v>
       </c>
       <c r="K39" t="n">
-        <v>23.81047453257899</v>
+        <v>20.62796989744321</v>
       </c>
     </row>
     <row r="40">
@@ -1916,16 +1916,16 @@
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>0.1706042457406765</v>
+        <v>0.1676256087337018</v>
       </c>
       <c r="I40" t="n">
-        <v>0.3684065372658357</v>
+        <v>0.3419947202577616</v>
       </c>
       <c r="J40" t="n">
-        <v>0.1149504511057552</v>
+        <v>0.1120999674151963</v>
       </c>
       <c r="K40" t="n">
-        <v>287.8072109054121</v>
+        <v>287.6755689883772</v>
       </c>
     </row>
     <row r="41">
@@ -1950,19 +1950,19 @@
         <v>0.1047526905620423</v>
       </c>
       <c r="G41" t="n">
-        <v>0.1519855807899402</v>
+        <v>0.1520714798578533</v>
       </c>
       <c r="H41" t="n">
-        <v>0.1343430341677353</v>
+        <v>0.1302772010310571</v>
       </c>
       <c r="I41" t="n">
-        <v>0.3242768006809282</v>
+        <v>0.2905532322932284</v>
       </c>
       <c r="J41" t="n">
-        <v>0.1186228365218494</v>
+        <v>0.1158682414242365</v>
       </c>
       <c r="K41" t="n">
-        <v>33.24996681138243</v>
+        <v>29.3570936468391</v>
       </c>
     </row>
     <row r="42">
@@ -1987,19 +1987,19 @@
         <v>0.1061432406569026</v>
       </c>
       <c r="G42" t="n">
-        <v>0.107472458961546</v>
+        <v>0.1074890784398424</v>
       </c>
       <c r="H42" t="n">
-        <v>0.1376314647229725</v>
+        <v>0.1331554864351283</v>
       </c>
       <c r="I42" t="n">
-        <v>0.3604284222101862</v>
+        <v>0.3303691604638617</v>
       </c>
       <c r="J42" t="n">
-        <v>0.120796816094503</v>
+        <v>0.1177479835913935</v>
       </c>
       <c r="K42" t="n">
-        <v>35.18395312068824</v>
+        <v>31.82603377152134</v>
       </c>
     </row>
     <row r="43">
@@ -2024,19 +2024,19 @@
         <v>0.05420715580231423</v>
       </c>
       <c r="G43" t="n">
-        <v>0.789498647860758</v>
+        <v>0.7901703435653683</v>
       </c>
       <c r="H43" t="n">
-        <v>0.0859447227882303</v>
+        <v>0.09105127523154673</v>
       </c>
       <c r="I43" t="n">
-        <v>0.1437040409630082</v>
+        <v>0.1317728078337646</v>
       </c>
       <c r="J43" t="n">
-        <v>0.06060569884473403</v>
+        <v>0.06174187641490887</v>
       </c>
       <c r="K43" t="n">
-        <v>22.97284903267187</v>
+        <v>21.50006017357976</v>
       </c>
     </row>
     <row r="44">
@@ -2061,19 +2061,19 @@
         <v>0.1237721026521449</v>
       </c>
       <c r="G44" t="n">
-        <v>0.3748591807359359</v>
+        <v>0.3751611555632425</v>
       </c>
       <c r="H44" t="n">
-        <v>0.2046226919158565</v>
+        <v>0.2122818678897395</v>
       </c>
       <c r="I44" t="n">
-        <v>0.3787278424993986</v>
+        <v>0.3436234607160102</v>
       </c>
       <c r="J44" t="n">
-        <v>0.1501956181769875</v>
+        <v>0.1504437808901598</v>
       </c>
       <c r="K44" t="n">
-        <v>44.93275205625682</v>
+        <v>41.37863585575949</v>
       </c>
     </row>
     <row r="45">
@@ -2098,19 +2098,19 @@
         <v>0.06517075743771605</v>
       </c>
       <c r="G45" t="n">
-        <v>0.2306291987242972</v>
+        <v>0.2307169350353097</v>
       </c>
       <c r="H45" t="n">
-        <v>0.0838453124325786</v>
+        <v>0.08263204119155582</v>
       </c>
       <c r="I45" t="n">
-        <v>0.1864409512365733</v>
+        <v>0.1670756976252482</v>
       </c>
       <c r="J45" t="n">
-        <v>0.07403402338739604</v>
+        <v>0.07310974437270988</v>
       </c>
       <c r="K45" t="n">
-        <v>20.06726124646968</v>
+        <v>17.61315680424924</v>
       </c>
     </row>
     <row r="46">
@@ -2135,19 +2135,19 @@
         <v>0.04965378614700133</v>
       </c>
       <c r="G46" t="n">
-        <v>0.5964504337034746</v>
+        <v>0.5965351648103498</v>
       </c>
       <c r="H46" t="n">
-        <v>0.06767199586071961</v>
+        <v>0.07006911208919454</v>
       </c>
       <c r="I46" t="n">
-        <v>0.1238606522538896</v>
+        <v>0.1108356701248033</v>
       </c>
       <c r="J46" t="n">
-        <v>0.05437309070680738</v>
+        <v>0.05492902015520439</v>
       </c>
       <c r="K46" t="n">
-        <v>19.78110553666146</v>
+        <v>18.15881593207973</v>
       </c>
     </row>
     <row r="47">
@@ -2172,19 +2172,19 @@
         <v>0.0416256384089698</v>
       </c>
       <c r="G47" t="n">
-        <v>1.339036172286537</v>
+        <v>1.338511021842968</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0656589813606389</v>
+        <v>0.07232183482085287</v>
       </c>
       <c r="I47" t="n">
-        <v>0.09385653101474643</v>
+        <v>0.09023779824501553</v>
       </c>
       <c r="J47" t="n">
-        <v>0.04070878921349885</v>
+        <v>0.04274727504976644</v>
       </c>
       <c r="K47" t="n">
-        <v>42.08364905744622</v>
+        <v>41.2898947625887</v>
       </c>
     </row>
     <row r="48">
@@ -2209,19 +2209,19 @@
         <v>0.03139402046797896</v>
       </c>
       <c r="G48" t="n">
-        <v>0.475286229635129</v>
+        <v>0.4755482927586865</v>
       </c>
       <c r="H48" t="n">
-        <v>0.04156999568865775</v>
+        <v>0.04298556888676133</v>
       </c>
       <c r="I48" t="n">
-        <v>0.07335443123557273</v>
+        <v>0.06489633386475928</v>
       </c>
       <c r="J48" t="n">
-        <v>0.03397497248047825</v>
+        <v>0.03424952972094435</v>
       </c>
       <c r="K48" t="n">
-        <v>11.12187887523656</v>
+        <v>10.20248991293702</v>
       </c>
     </row>
     <row r="49">
@@ -2246,19 +2246,19 @@
         <v>0.087074436583873</v>
       </c>
       <c r="G49" t="n">
-        <v>0.2416883040454638</v>
+        <v>0.2418808229664635</v>
       </c>
       <c r="H49" t="n">
-        <v>0.1099672004100175</v>
+        <v>0.1093265298930782</v>
       </c>
       <c r="I49" t="n">
-        <v>0.23646931023226</v>
+        <v>0.2076740232293291</v>
       </c>
       <c r="J49" t="n">
-        <v>0.09544167336386078</v>
+        <v>0.09452271156425596</v>
       </c>
       <c r="K49" t="n">
-        <v>26.70343328875996</v>
+        <v>23.32917765215249</v>
       </c>
     </row>
     <row r="50">
@@ -2283,19 +2283,19 @@
         <v>0.05683484063202682</v>
       </c>
       <c r="G50" t="n">
-        <v>0.5094439136645887</v>
+        <v>0.5097543576753807</v>
       </c>
       <c r="H50" t="n">
-        <v>0.09517692442419252</v>
+        <v>0.1018087141339633</v>
       </c>
       <c r="I50" t="n">
-        <v>0.16991439962817</v>
+        <v>0.1619034574224135</v>
       </c>
       <c r="J50" t="n">
-        <v>0.06535162366870631</v>
+        <v>0.0667782892278581</v>
       </c>
       <c r="K50" t="n">
-        <v>21.79934058714741</v>
+        <v>20.96964050837762</v>
       </c>
     </row>
     <row r="51">
@@ -2320,19 +2320,19 @@
         <v>0.0505186818866572</v>
       </c>
       <c r="G51" t="n">
-        <v>0.9236125516784897</v>
+        <v>0.9234564953019193</v>
       </c>
       <c r="H51" t="n">
-        <v>0.08326600045975879</v>
+        <v>0.09007778742194845</v>
       </c>
       <c r="I51" t="n">
-        <v>0.1273683862937707</v>
+        <v>0.1208476890716082</v>
       </c>
       <c r="J51" t="n">
-        <v>0.05443018347392521</v>
+        <v>0.05628567948460878</v>
       </c>
       <c r="K51" t="n">
-        <v>20.30704845469804</v>
+        <v>19.29316191553713</v>
       </c>
     </row>
     <row r="52">
@@ -2357,19 +2357,19 @@
         <v>0.05168196383903029</v>
       </c>
       <c r="G52" t="n">
-        <v>1.283588449695047</v>
+        <v>1.280945302857047</v>
       </c>
       <c r="H52" t="n">
-        <v>0.1193211919174486</v>
+        <v>0.1314827956834052</v>
       </c>
       <c r="I52" t="n">
-        <v>0.1529227739626812</v>
+        <v>0.1535215558412565</v>
       </c>
       <c r="J52" t="n">
-        <v>0.06030474992278908</v>
+        <v>0.06330591556033345</v>
       </c>
       <c r="K52" t="n">
-        <v>30.88005741598262</v>
+        <v>31.30391010566217</v>
       </c>
     </row>
     <row r="53">
@@ -2394,19 +2394,19 @@
         <v>0.08968398826331808</v>
       </c>
       <c r="G53" t="n">
-        <v>0.2347833936932623</v>
+        <v>0.2349398152284717</v>
       </c>
       <c r="H53" t="n">
-        <v>0.1195221312647571</v>
+        <v>0.1195607732583423</v>
       </c>
       <c r="I53" t="n">
-        <v>0.2494612139124117</v>
+        <v>0.2225573355298108</v>
       </c>
       <c r="J53" t="n">
-        <v>0.1027796986504039</v>
+        <v>0.1018493936640175</v>
       </c>
       <c r="K53" t="n">
-        <v>27.46135539421528</v>
+        <v>23.97805036504562</v>
       </c>
     </row>
     <row r="54">
@@ -2431,19 +2431,19 @@
         <v>0.05422586004700646</v>
       </c>
       <c r="G54" t="n">
-        <v>0.788617771364811</v>
+        <v>0.789424268479189</v>
       </c>
       <c r="H54" t="n">
-        <v>0.08624195009105211</v>
+        <v>0.09140558857921302</v>
       </c>
       <c r="I54" t="n">
-        <v>0.1442220089767</v>
+        <v>0.1327787353859856</v>
       </c>
       <c r="J54" t="n">
-        <v>0.06075760145905176</v>
+        <v>0.06193108976384032</v>
       </c>
       <c r="K54" t="n">
-        <v>22.99747975411427</v>
+        <v>21.57749491001278</v>
       </c>
     </row>
     <row r="55">
@@ -2468,19 +2468,19 @@
         <v>0.0918153615746328</v>
       </c>
       <c r="G55" t="n">
-        <v>0.1719890625120795</v>
+        <v>0.1721109392595936</v>
       </c>
       <c r="H55" t="n">
-        <v>0.1181472179666918</v>
+        <v>0.1152802976569558</v>
       </c>
       <c r="I55" t="n">
-        <v>0.2719506160155061</v>
+        <v>0.2421459571753845</v>
       </c>
       <c r="J55" t="n">
-        <v>0.1042204969475328</v>
+        <v>0.1020960656696733</v>
       </c>
       <c r="K55" t="n">
-        <v>29.82104485393026</v>
+        <v>26.15871746972064</v>
       </c>
     </row>
     <row r="56">
@@ -2505,19 +2505,19 @@
         <v>0.06089031740564841</v>
       </c>
       <c r="G56" t="n">
-        <v>0.3777253460517036</v>
+        <v>0.3780293943245303</v>
       </c>
       <c r="H56" t="n">
-        <v>0.08875102137242051</v>
+        <v>0.09142469304847899</v>
       </c>
       <c r="I56" t="n">
-        <v>0.1677264675228566</v>
+        <v>0.1501235612973651</v>
       </c>
       <c r="J56" t="n">
-        <v>0.0703608096680559</v>
+        <v>0.07051988823836702</v>
       </c>
       <c r="K56" t="n">
-        <v>19.8886152169165</v>
+        <v>17.61275657097954</v>
       </c>
     </row>
     <row r="57">
@@ -2542,19 +2542,19 @@
         <v>0.05441577072811794</v>
       </c>
       <c r="G57" t="n">
-        <v>0.7302289528715716</v>
+        <v>0.7307333293952066</v>
       </c>
       <c r="H57" t="n">
-        <v>0.09145362400365933</v>
+        <v>0.09807685812267332</v>
       </c>
       <c r="I57" t="n">
-        <v>0.1468387739365015</v>
+        <v>0.1360802948355526</v>
       </c>
       <c r="J57" t="n">
-        <v>0.06182932255866344</v>
+        <v>0.06335488052811143</v>
       </c>
       <c r="K57" t="n">
-        <v>23.32119296945787</v>
+        <v>21.99392869109058</v>
       </c>
     </row>
     <row r="58">
@@ -2579,19 +2579,19 @@
         <v>0.05413871220190486</v>
       </c>
       <c r="G58" t="n">
-        <v>1.224161851104613</v>
+        <v>1.223206665621724</v>
       </c>
       <c r="H58" t="n">
-        <v>0.1101630356952656</v>
+        <v>0.121559872038679</v>
       </c>
       <c r="I58" t="n">
-        <v>0.1498095527679877</v>
+        <v>0.1459562101869914</v>
       </c>
       <c r="J58" t="n">
-        <v>0.06049536187709915</v>
+        <v>0.06344003360637805</v>
       </c>
       <c r="K58" t="n">
-        <v>33.33352633689532</v>
+        <v>32.88358309425137</v>
       </c>
     </row>
     <row r="59">
@@ -2616,19 +2616,19 @@
         <v>0.07957998521258956</v>
       </c>
       <c r="G59" t="n">
-        <v>1.538917153961179</v>
+        <v>1.544641537029146</v>
       </c>
       <c r="H59" t="n">
-        <v>0.1201758186720678</v>
+        <v>0.1302690168927967</v>
       </c>
       <c r="I59" t="n">
-        <v>0.1797840977461756</v>
+        <v>0.172598818248863</v>
       </c>
       <c r="J59" t="n">
-        <v>0.07724338387776326</v>
+        <v>0.08031721253026598</v>
       </c>
       <c r="K59" t="n">
-        <v>101.2563905635704</v>
+        <v>100.5742702108438</v>
       </c>
     </row>
     <row r="60">
@@ -2653,19 +2653,19 @@
         <v>0.09186622969397451</v>
       </c>
       <c r="G60" t="n">
-        <v>2.199483705235565</v>
+        <v>2.206924424350894</v>
       </c>
       <c r="H60" t="n">
-        <v>0.2046686449674033</v>
+        <v>0.2297703732538908</v>
       </c>
       <c r="I60" t="n">
-        <v>0.2501802427306528</v>
+        <v>0.2556131731941947</v>
       </c>
       <c r="J60" t="n">
-        <v>0.09112766868662205</v>
+        <v>0.09780710105275116</v>
       </c>
       <c r="K60" t="n">
-        <v>192.3826452374905</v>
+        <v>192.4953669938859</v>
       </c>
     </row>
     <row r="61">
@@ -2690,19 +2690,19 @@
         <v>0.1069199762361368</v>
       </c>
       <c r="G61" t="n">
-        <v>3.04881298535346</v>
+        <v>3.036990597498759</v>
       </c>
       <c r="H61" t="n">
-        <v>0.2884758767250113</v>
+        <v>0.3254311497196966</v>
       </c>
       <c r="I61" t="n">
-        <v>0.3284019170155369</v>
+        <v>0.3445339391625824</v>
       </c>
       <c r="J61" t="n">
-        <v>0.108165788306071</v>
+        <v>0.1178987443708941</v>
       </c>
       <c r="K61" t="n">
-        <v>287.7882631074611</v>
+        <v>288.4478030298091</v>
       </c>
     </row>
     <row r="62">
@@ -2727,19 +2727,19 @@
         <v>0.1160306569847246</v>
       </c>
       <c r="G62" t="n">
-        <v>3.902628952874985</v>
+        <v>3.861588237940931</v>
       </c>
       <c r="H62" t="n">
-        <v>8.812300595121476</v>
+        <v>0.3723372536716586</v>
       </c>
       <c r="I62" t="n">
-        <v>8.234964100988691</v>
+        <v>0.3940723355764426</v>
       </c>
       <c r="J62" t="n">
-        <v>2.082009142850571</v>
+        <v>0.124843437616209</v>
       </c>
       <c r="K62" t="n">
-        <v>12807.26522110153</v>
+        <v>372.7943381155987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>